<commit_message>
Correção de bug no upload da planilha
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\bkp-usuarios\nilson\Desktop\Capgemini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\bkp-usuarios\nilson\Desktop\teste-tecnico-capgemini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6BBFA3-DE83-4A74-9334-58BF11AB5BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91C48B23-903A-4A81-B8B4-3A769BA9862B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D9C88F38-B4E9-4F33-8DA4-F4AC2F42F675}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AD112442-60D1-4A49-872B-B8536D7167CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,31 +27,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
+    <t>Descrição 1</t>
+  </si>
+  <si>
+    <t>Descrição 2</t>
+  </si>
+  <si>
+    <t>Descrição 3</t>
+  </si>
+  <si>
+    <t>Descrição 4</t>
+  </si>
+  <si>
+    <t>Descrição 5</t>
+  </si>
+  <si>
+    <t>Descrição 6</t>
+  </si>
+  <si>
+    <t>Descrição 7</t>
+  </si>
+  <si>
+    <t>Descrição 8</t>
+  </si>
+  <si>
     <t>Descrição 9</t>
-  </si>
-  <si>
-    <t>Descrição 1</t>
-  </si>
-  <si>
-    <t>Descrição 2</t>
-  </si>
-  <si>
-    <t>Descrição 3</t>
-  </si>
-  <si>
-    <t>Descrição 4</t>
-  </si>
-  <si>
-    <t>Descrição 5</t>
-  </si>
-  <si>
-    <t>Descrição 6</t>
-  </si>
-  <si>
-    <t>Descrição 7</t>
-  </si>
-  <si>
-    <t>Descrição 8</t>
   </si>
 </sst>
 </file>
@@ -93,8 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -410,158 +409,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78C68A7-4FA0-4E17-A95D-69FFA790900A}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964A99EA-D26E-4BEB-9945-F687B0D0B679}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D1" sqref="D1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>44131</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>44163</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>44163</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44195</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44195</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44227</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>44227</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44259</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>44259</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44291</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>44291</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1">
-        <v>15.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>44323</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>44355</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44387</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>44387</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>9</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>